<commit_message>
adding client payment payment type
</commit_message>
<xml_diff>
--- a/resources/import/client_payment_report.xlsx
+++ b/resources/import/client_payment_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Policy #</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -315,6 +318,7 @@
     <col customWidth="1" min="5" max="5" width="18.0"/>
     <col customWidth="1" min="6" max="6" width="18.38"/>
     <col customWidth="1" min="7" max="7" width="20.0"/>
+    <col customWidth="1" min="8" max="8" width="22.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -339,6 +343,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>